<commit_message>
RTTBC24 Draft #2 Countdown Timer Enabled
</commit_message>
<xml_diff>
--- a/calendar-import-files/Michael-Casserly-Gallop-Draft-Tasks-for-Google-Calendar.xlsx
+++ b/calendar-import-files/Michael-Casserly-Gallop-Draft-Tasks-for-Google-Calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/299f8723705ec823/Webmaster/gallop-racing.com/calendar-import-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{17A1D9B9-8994-4361-99E0-CCA1520F2178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE1E3F88-FC4B-4781-A77C-25A8A058B1F6}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="8_{17A1D9B9-8994-4361-99E0-CCA1520F2178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F318B5A6-75DC-4392-AE58-E5005A245586}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{27DBC710-212C-4B60-B927-B9EE36866F81}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Subject</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>League Sheet &gt; Import Stables Sheet &gt; Confirm there are no Red Flags in Columns A, D, E, and F, and for any Horse Name Columns in Subsequent Drafts</t>
+  </si>
+  <si>
+    <t>Turn on Draft Countdown Timer</t>
+  </si>
+  <si>
+    <t>Turn off Draft Countdown Timer</t>
   </si>
 </sst>
 </file>
@@ -480,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{284028C9-2345-4A3E-B3AE-70C83AECA38B}">
-  <dimension ref="A1:H171"/>
+  <dimension ref="A1:H173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,19 +572,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1">
-        <v>45470</v>
+        <v>45468</v>
       </c>
       <c r="C4" s="3">
-        <v>0.875</v>
+        <v>0.375</v>
       </c>
       <c r="D4" s="1">
-        <v>45470</v>
+        <v>45468</v>
       </c>
       <c r="E4" s="3">
-        <v>0.91666666666666663</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -586,16 +592,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1">
-        <v>45471</v>
+        <v>45470</v>
       </c>
       <c r="C5" s="3">
         <v>0.875</v>
       </c>
       <c r="D5" s="1">
-        <v>45471</v>
+        <v>45470</v>
       </c>
       <c r="E5" s="3">
         <v>0.91666666666666663</v>
@@ -606,19 +612,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1">
-        <v>45472</v>
+        <v>45471</v>
       </c>
       <c r="C6" s="3">
-        <v>0.45833333333333331</v>
+        <v>0.875</v>
       </c>
       <c r="D6" s="1">
-        <v>45472</v>
+        <v>45471</v>
       </c>
       <c r="E6" s="3">
-        <v>0.5</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -626,30 +632,27 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1">
         <v>45472</v>
       </c>
       <c r="C7" s="3">
-        <v>0.41666666666666669</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="D7" s="1">
         <v>45472</v>
       </c>
       <c r="E7" s="3">
-        <v>0.45833333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
       </c>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1">
         <v>45472</v>
@@ -669,39 +672,42 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>45472</v>
       </c>
       <c r="C9" s="3">
-        <v>0.5</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="D9" s="1">
         <v>45472</v>
       </c>
       <c r="E9" s="3">
-        <v>0.54166666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
       </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1">
-        <v>45474</v>
+        <v>45472</v>
       </c>
       <c r="C10" s="3">
-        <v>0.70833333333333337</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="D10" s="1">
-        <v>45474</v>
+        <v>45472</v>
       </c>
       <c r="E10" s="3">
-        <v>0.83333333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -709,19 +715,19 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1">
-        <v>45474</v>
+        <v>45472</v>
       </c>
       <c r="C11" s="3">
-        <v>0.83333333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="D11" s="1">
-        <v>45474</v>
+        <v>45472</v>
       </c>
       <c r="E11" s="3">
-        <v>0.875</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -729,31 +735,63 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1">
         <v>45474</v>
       </c>
       <c r="C12" s="3">
-        <v>0.875</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="D12" s="1">
         <v>45474</v>
       </c>
       <c r="E12" s="3">
-        <v>0.91666666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45474</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D13" s="1">
+        <v>45474</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45474</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="D14" s="1">
+        <v>45474</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
@@ -786,7 +824,6 @@
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="H22" s="2"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
@@ -795,6 +832,7 @@
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="D24" s="1"/>
+      <c r="H24" s="2"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
@@ -847,16 +885,15 @@
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="D37" s="1"/>
-      <c r="H37" s="2"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="D38" s="1"/>
-      <c r="H38" s="2"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="D39" s="1"/>
+      <c r="H39" s="2"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
@@ -866,15 +903,16 @@
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="H41" s="2"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="D42" s="1"/>
+      <c r="H42" s="2"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="D43" s="1"/>
+      <c r="H43" s="2"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
@@ -1216,71 +1254,69 @@
       <c r="B128" s="1"/>
       <c r="D128" s="1"/>
     </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B129" s="1"/>
       <c r="D129" s="1"/>
     </row>
-    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="1"/>
       <c r="D130" s="1"/>
     </row>
-    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B131" s="1"/>
       <c r="D131" s="1"/>
     </row>
-    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132" s="1"/>
       <c r="D132" s="1"/>
     </row>
-    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B133" s="1"/>
       <c r="D133" s="1"/>
     </row>
-    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B134" s="1"/>
       <c r="D134" s="1"/>
     </row>
-    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B135" s="1"/>
       <c r="D135" s="1"/>
     </row>
-    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B136" s="1"/>
       <c r="D136" s="1"/>
     </row>
-    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B137" s="1"/>
       <c r="D137" s="1"/>
     </row>
-    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B138" s="1"/>
       <c r="D138" s="1"/>
     </row>
-    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B139" s="1"/>
       <c r="D139" s="1"/>
     </row>
-    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B140" s="1"/>
       <c r="D140" s="1"/>
     </row>
-    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B141" s="1"/>
       <c r="D141" s="1"/>
     </row>
-    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B142" s="1"/>
       <c r="D142" s="1"/>
     </row>
-    <row r="143" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B143" s="1"/>
       <c r="D143" s="1"/>
-      <c r="H143" s="2"/>
-    </row>
-    <row r="144" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B144" s="1"/>
       <c r="D144" s="1"/>
-      <c r="H144" s="2"/>
     </row>
     <row r="145" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B145" s="1"/>
@@ -1290,10 +1326,12 @@
     <row r="146" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B146" s="1"/>
       <c r="D146" s="1"/>
+      <c r="H146" s="2"/>
     </row>
     <row r="147" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B147" s="1"/>
       <c r="D147" s="1"/>
+      <c r="H147" s="2"/>
     </row>
     <row r="148" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B148" s="1"/>
@@ -1310,20 +1348,20 @@
     <row r="151" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B151" s="1"/>
       <c r="D151" s="1"/>
-      <c r="H151" s="2"/>
     </row>
     <row r="152" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B152" s="1"/>
       <c r="D152" s="1"/>
-      <c r="H152" s="2"/>
     </row>
     <row r="153" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B153" s="1"/>
       <c r="D153" s="1"/>
+      <c r="H153" s="2"/>
     </row>
     <row r="154" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B154" s="1"/>
       <c r="D154" s="1"/>
+      <c r="H154" s="2"/>
     </row>
     <row r="155" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B155" s="1"/>
@@ -1336,7 +1374,6 @@
     <row r="157" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B157" s="1"/>
       <c r="D157" s="1"/>
-      <c r="H157" s="2"/>
     </row>
     <row r="158" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B158" s="1"/>
@@ -1345,6 +1382,7 @@
     <row r="159" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B159" s="1"/>
       <c r="D159" s="1"/>
+      <c r="H159" s="2"/>
     </row>
     <row r="160" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B160" s="1"/>
@@ -1393,6 +1431,14 @@
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="1"/>
       <c r="D171" s="1"/>
+    </row>
+    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B172" s="1"/>
+      <c r="D172" s="1"/>
+    </row>
+    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B173" s="1"/>
+      <c r="D173" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>